<commit_message>
Updated C3DC phs002371 input query
</commit_message>
<xml_diff>
--- a/InputFiles/C3DC/TC01_C3DC_phs001437_SexAtBirth-Unknown.xlsx
+++ b/InputFiles/C3DC/TC01_C3DC_phs001437_SexAtBirth-Unknown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sohilz2/Automation/poc-11-27-2024/Commons_Automation/InputFiles/C3DC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CA19E58-0513-394B-B601-427C99DC6A2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA35127-6094-A546-9EB4-463869A672CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="35840" yWindow="-2240" windowWidth="30240" windowHeight="24500" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -288,7 +288,7 @@
 LEFT JOIN 
     df_reference_files rfs ON std.id = rfs."study.id"
 WHERE 
-    std.dbgap_accession = 'phs001437' AND prt.sex_at_birth = 'Unknown'
+    std.dbgap_accession = 'phs001437' AND prt.sex_at_birth = 'Unknown' AND trt.treatment_id IS NOT NULL
 ORDER BY 
     prt.participant_id ASC
 LIMIT 100;</t>
@@ -298,9 +298,23 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -353,11 +367,17 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -683,7 +703,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -720,7 +740,7 @@
       <c r="B2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D2" t="s">
@@ -751,7 +771,7 @@
       <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="2"/>
@@ -782,7 +802,7 @@
       <c r="C9" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added C3DC phs001437 to Smoke suite
</commit_message>
<xml_diff>
--- a/InputFiles/C3DC/TC01_C3DC_phs001437_SexAtBirth-Unknown.xlsx
+++ b/InputFiles/C3DC/TC01_C3DC_phs001437_SexAtBirth-Unknown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sohilz2/Automation/poc-11-27-2024/Commons_Automation/InputFiles/C3DC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA35127-6094-A546-9EB4-463869A672CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF8C19F2-B634-894A-93AD-68979095FD94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="35840" yWindow="-2240" windowWidth="30240" windowHeight="24500" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -271,7 +271,7 @@
         trt.age_at_treatment_end 
 END AS "Age at Treatment End",
     trt.treatment_type AS "Treatment Type",
-    CONCAT(REPLACE(trt.treatment_agent, ';', ', ')) AS "Treatment Agent",
+    REPLACE(trt.treatment_agent, ';', ', ') AS "Treatment Agent",
     std.dbgap_accession AS "dbGaP Accession"
 FROM 
     df_study std

</xml_diff>